<commit_message>
Se agrega columna de unidades de los parametros.
</commit_message>
<xml_diff>
--- a/Programas/PARAMETROS ACIDWASH.xlsx
+++ b/Programas/PARAMETROS ACIDWASH.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>PARAMETROS</t>
   </si>
@@ -78,13 +78,7 @@
     <t>Segundos</t>
   </si>
   <si>
-    <t>UNIDADES</t>
-  </si>
-  <si>
-    <t>DESCRIPCION</t>
-  </si>
-  <si>
-    <t>BLOQUE</t>
+    <t>Unidades</t>
   </si>
 </sst>
 </file>
@@ -161,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -184,9 +178,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -493,18 +484,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E19"/>
+  <dimension ref="B1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E13"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
     <col min="3" max="3" width="3.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="44.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -527,152 +518,141 @@
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="E4" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>20</v>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>19</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
+      <c r="B11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="2:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="2:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="7" t="s">
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="2:5" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="2:5" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B4:D4"/>
     <mergeCell ref="B1:E2"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
     <mergeCell ref="B15:E15"/>
   </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega manual de usuario.
</commit_message>
<xml_diff>
--- a/Programas/PARAMETROS ACIDWASH.xlsx
+++ b/Programas/PARAMETROS ACIDWASH.xlsx
@@ -57,9 +57,6 @@
     <t>Selector de manual/automatico en manual:</t>
   </si>
   <si>
-    <t>Al presionar el boton MARCHA comienza a correr el tiempo de proceso (default 600seg), y hace que la tombola inicie con la pausa de rotacion, comienza a girar hacia un sentido por el tiempo de rotacion (default 60seg), pare por el tiempo de pausa (7seg), comienze a girar en el otro sentido, y continua repitiendo la secuencia hasta que se termine el tiempo de proceso o se presione el paro de emergencia.</t>
-  </si>
-  <si>
     <t>B69</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Unidades</t>
+  </si>
+  <si>
+    <t>Al presionar el boton MARCHA comienza a correr el tiempo de proceso (default 600seg), y hace que la tombola comience a girar hacia un sentido por el tiempo de rotacion (default 60seg), pare por el tiempo de pausa (7seg), comienze a girar en el otro sentido, y continua repitiendo la secuencia hasta que se termine el tiempo de proceso o se presione el paro de emergencia.</t>
   </si>
 </sst>
 </file>
@@ -174,14 +174,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,174 +484,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E18"/>
+  <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="3.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="2:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="2:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+    </row>
+    <row r="13" spans="2:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="2:5" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="2:4" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B1:E2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="50" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>